<commit_message>
Criação do arquivo de input de dados e mapeamento na estrutura do curriculo
</commit_message>
<xml_diff>
--- a/dados_exemplo.xlsx
+++ b/dados_exemplo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GABRIEL\Documents\curriculo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8955BBE9-0DEA-4231-B7E5-43A6D4E3C952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7008A3-DDBF-4E84-802C-FF1B1DBAB789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{8D5C2EF7-12FE-4554-BA32-BDC8432EB3A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{8D5C2EF7-12FE-4554-BA32-BDC8432EB3A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Cabeçalho" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="233">
   <si>
     <t>Nome</t>
   </si>
@@ -707,6 +707,39 @@
   </si>
   <si>
     <t>Bachelor in Systems Engineering</t>
+  </si>
+  <si>
+    <t>nov</t>
+  </si>
+  <si>
+    <t>eco</t>
+  </si>
+  <si>
+    <t>yop</t>
+  </si>
+  <si>
+    <t>luna</t>
+  </si>
+  <si>
+    <t>aqn</t>
+  </si>
+  <si>
+    <t>pipa</t>
+  </si>
+  <si>
+    <t>grad</t>
+  </si>
+  <si>
+    <t>mic</t>
+  </si>
+  <si>
+    <t>fer</t>
+  </si>
+  <si>
+    <t>csap</t>
+  </si>
+  <si>
+    <t>agil</t>
   </si>
 </sst>
 </file>
@@ -1516,255 +1549,276 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BF54007-237F-4FC1-9763-EE9491EC144F}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="10"/>
-    <col min="3" max="3" width="48.42578125" style="11" customWidth="1"/>
-    <col min="4" max="6" width="9.140625" style="10"/>
-    <col min="7" max="7" width="14.28515625" style="11" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="3" width="9.140625" style="10"/>
+    <col min="4" max="4" width="48.42578125" style="11" customWidth="1"/>
+    <col min="5" max="7" width="9.140625" style="10"/>
+    <col min="8" max="8" width="14.28515625" style="11" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A2" s="10">
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="E2" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="E2" s="10">
+      <c r="F2" s="10">
         <v>2024</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="G2" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>127</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>116</v>
       </c>
       <c r="I2" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="K2" s="10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="17.25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A3" s="10">
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>118</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="F3" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="G3" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>128</v>
-      </c>
-      <c r="H3" t="s">
-        <v>118</v>
       </c>
       <c r="I3" t="s">
         <v>118</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" t="s">
+        <v>118</v>
+      </c>
+      <c r="K3" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="17.25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A4" s="10">
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="E4" s="14">
+      <c r="F4" s="14">
         <v>2022</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="G4" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>129</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>120</v>
       </c>
       <c r="I4" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="K4" s="10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="17.25" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A5" s="10">
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="F5" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="G5" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>130</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>117</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>117</v>
       </c>
       <c r="J5" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="K5" s="10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="17.25" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A6" s="10">
         <v>6</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="E6" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="E6" s="10">
+      <c r="F6" s="10">
         <v>2019</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="G6" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>110</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>121</v>
       </c>
       <c r="I6" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="K6" s="10" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="17.25" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A7" s="10">
         <v>7</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="E7" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>131</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>119</v>
       </c>
       <c r="I7" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="K7" s="10" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="C9" s="12"/>
-    </row>
-    <row r="11" spans="1:11" ht="17.25" x14ac:dyDescent="0.4">
-      <c r="C11" s="9"/>
-      <c r="G11" s="10"/>
-      <c r="J11"/>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="D9" s="12"/>
+    </row>
+    <row r="11" spans="1:12" ht="17.25" x14ac:dyDescent="0.4">
+      <c r="D11" s="9"/>
+      <c r="H11" s="10"/>
+      <c r="K11"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1773,231 +1827,250 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9D50774-E0FE-44E9-B03C-E8852FD49129}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.140625" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.140625" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
       <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
         <v>89</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>90</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>91</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>92</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>93</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>94</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>95</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C2" t="s">
         <v>220</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>188</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>189</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>52</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>190</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>2020</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>206</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="H3" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>2020</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>200</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" t="s">
+        <v>230</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="H4" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="I4" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>201</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" t="s">
+        <v>231</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>2017</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>205</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="H5" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <v>2017</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>202</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" t="s">
+        <v>232</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>204</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="H6" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="I6" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>203</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D12" s="3"/>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E12" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Mudanças no design e inserção de detalhamento de atividades em formações e experiências
</commit_message>
<xml_diff>
--- a/dados_exemplo.xlsx
+++ b/dados_exemplo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GABRIEL\Documents\curriculo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7008A3-DDBF-4E84-802C-FF1B1DBAB789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8397395D-F18E-4A49-AB22-F4FA110E749F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{8D5C2EF7-12FE-4554-BA32-BDC8432EB3A7}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="245">
   <si>
     <t>Nome</t>
   </si>
@@ -740,13 +740,49 @@
   </si>
   <si>
     <t>agil</t>
+  </si>
+  <si>
+    <t>Desenvolvimento</t>
+  </si>
+  <si>
+    <t>Testes de Integração</t>
+  </si>
+  <si>
+    <t>Melhoria em 14% da performance</t>
+  </si>
+  <si>
+    <t>Testes de segurança</t>
+  </si>
+  <si>
+    <t>detalhe_1</t>
+  </si>
+  <si>
+    <t>detalhe_2</t>
+  </si>
+  <si>
+    <t>detalhe_3</t>
+  </si>
+  <si>
+    <t>detalhe_4</t>
+  </si>
+  <si>
+    <t>detalhe_5</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -848,6 +884,12 @@
       <color theme="1"/>
       <name val="Trebuchet MS"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1549,10 +1591,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BF54007-237F-4FC1-9763-EE9491EC144F}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="L13" sqref="L13:M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.4"/>
@@ -1564,7 +1606,7 @@
     <col min="9" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A1" s="10" t="s">
         <v>12</v>
       </c>
@@ -1601,8 +1643,23 @@
       <c r="L1" s="10" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="17.25" x14ac:dyDescent="0.4">
+      <c r="M1" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -1636,8 +1693,20 @@
       <c r="K2" s="10" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="17.25" x14ac:dyDescent="0.4">
+      <c r="M2" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A3" s="10">
         <v>2</v>
       </c>
@@ -1672,7 +1741,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="17.25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:17" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A4" s="10">
         <v>3</v>
       </c>
@@ -1707,7 +1776,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="17.25" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:17" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A5" s="10">
         <v>4</v>
       </c>
@@ -1742,7 +1811,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="17.25" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:17" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A6" s="10">
         <v>6</v>
       </c>
@@ -1776,8 +1845,14 @@
       <c r="K6" s="10" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="17.25" x14ac:dyDescent="0.4">
+      <c r="M6" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A7" s="10">
         <v>7</v>
       </c>
@@ -1812,25 +1887,26 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
       <c r="D9" s="12"/>
     </row>
-    <row r="11" spans="1:12" ht="17.25" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:17" ht="17.25" x14ac:dyDescent="0.4">
       <c r="D11" s="9"/>
       <c r="H11" s="10"/>
       <c r="K11"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9D50774-E0FE-44E9-B03C-E8852FD49129}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1844,7 +1920,7 @@
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1878,8 +1954,23 @@
       <c r="K1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="L1" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1914,10 +2005,13 @@
         <v>190</v>
       </c>
       <c r="L2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+      <c r="M2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1952,10 +2046,10 @@
         <v>200</v>
       </c>
       <c r="L3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1993,7 +2087,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2031,7 +2125,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2069,7 +2163,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E12" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de área de resumo, inserção da opção de comentário, parametrização do cabeçalho
</commit_message>
<xml_diff>
--- a/dados_exemplo.xlsx
+++ b/dados_exemplo.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GABRIEL\Documents\curriculo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE85BC7-B99C-4B08-8EB4-AD2169F8E599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C973BC45-9F69-461D-93A7-DEC2A3D60818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{8D5C2EF7-12FE-4554-BA32-BDC8432EB3A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{8D5C2EF7-12FE-4554-BA32-BDC8432EB3A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Cabeçalho" sheetId="1" r:id="rId1"/>
     <sheet name="Resumo" sheetId="8" r:id="rId2"/>
-    <sheet name="Seções" sheetId="6" r:id="rId3"/>
-    <sheet name="Experiências" sheetId="2" r:id="rId4"/>
-    <sheet name="Formações" sheetId="3" r:id="rId5"/>
-    <sheet name="Habilidades" sheetId="4" r:id="rId6"/>
-    <sheet name="Classes" sheetId="7" r:id="rId7"/>
+    <sheet name="Outros" sheetId="9" r:id="rId3"/>
+    <sheet name="Seções" sheetId="6" r:id="rId4"/>
+    <sheet name="Experiências" sheetId="2" r:id="rId5"/>
+    <sheet name="Formações" sheetId="3" r:id="rId6"/>
+    <sheet name="Habilidades" sheetId="4" r:id="rId7"/>
+    <sheet name="Classes" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="261">
   <si>
     <t>Nome</t>
   </si>
@@ -50,9 +51,6 @@
     <t>nome</t>
   </si>
   <si>
-    <t>título</t>
-  </si>
-  <si>
     <t>cidade</t>
   </si>
   <si>
@@ -71,9 +69,6 @@
     <t xml:space="preserve">MG </t>
   </si>
   <si>
-    <t>chave</t>
-  </si>
-  <si>
     <t>Desenvolvedor Back End como Freelancer</t>
   </si>
   <si>
@@ -89,9 +84,6 @@
     <t>tipo</t>
   </si>
   <si>
-    <t>principal</t>
-  </si>
-  <si>
     <t>2018 - 2019</t>
   </si>
   <si>
@@ -101,9 +93,6 @@
     <t>Desenvolvimento de um sistema de controle de estoque de uma empresa de locação de equipamentos de TI usando PHP e MySQL.</t>
   </si>
   <si>
-    <t>complementar</t>
-  </si>
-  <si>
     <t>classe</t>
   </si>
   <si>
@@ -362,9 +351,6 @@
     <t>OTHER PROFESSIONAL ACTIVITIES</t>
   </si>
   <si>
-    <t>secundária</t>
-  </si>
-  <si>
     <t>Update of a legacy system for managing buffalo registration, reproduction, and certification built using the CodeIgniter framework, MySQL, and PH</t>
   </si>
   <si>
@@ -749,30 +735,12 @@
     <t>Testes de segurança</t>
   </si>
   <si>
-    <t>detalhe_1</t>
-  </si>
-  <si>
-    <t>detalhe_2</t>
-  </si>
-  <si>
-    <t>detalhe_3</t>
-  </si>
-  <si>
-    <t>detalhe_4</t>
-  </si>
-  <si>
-    <t>detalhe_5</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
     <t>b</t>
   </si>
   <si>
-    <t>c</t>
-  </si>
-  <si>
     <t>texto_pt</t>
   </si>
   <si>
@@ -789,6 +757,75 @@
   </si>
   <si>
     <t>I am a full stack developer who has extensive experience in the complete systems development cycle</t>
+  </si>
+  <si>
+    <t>duracao</t>
+  </si>
+  <si>
+    <t>vol</t>
+  </si>
+  <si>
+    <t>Voluntariado 4h por dia na APAE de minha cidade</t>
+  </si>
+  <si>
+    <t>Work 4h a day as a Volunteer in the institution "APAE" in my my city</t>
+  </si>
+  <si>
+    <t>outros</t>
+  </si>
+  <si>
+    <t>OUTRAS INFORMAÇÕES</t>
+  </si>
+  <si>
+    <t>ADDITIONAL INFORMATION</t>
+  </si>
+  <si>
+    <t>Portifólio</t>
+  </si>
+  <si>
+    <t>Github</t>
+  </si>
+  <si>
+    <t>https://www.github.com/glouvss</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>titulo</t>
+  </si>
+  <si>
+    <t>detalhe_1_pt</t>
+  </si>
+  <si>
+    <t>detalhe_2_pt</t>
+  </si>
+  <si>
+    <t>detalhe_3_pt</t>
+  </si>
+  <si>
+    <t>detalhe_4_pt</t>
+  </si>
+  <si>
+    <t>detalhe_5_pt</t>
+  </si>
+  <si>
+    <t>detalhe_1_en</t>
+  </si>
+  <si>
+    <t>detalhe_2_en</t>
+  </si>
+  <si>
+    <t>detalhe_3_en</t>
+  </si>
+  <si>
+    <t>detalhe_4_en</t>
+  </si>
+  <si>
+    <t>detalhe_5_en</t>
+  </si>
+  <si>
+    <t>main</t>
   </si>
 </sst>
 </file>
@@ -1292,10 +1329,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01DA8488-C559-41A8-B6D7-36686CD06534}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1306,19 +1343,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1329,132 +1366,149 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="E2" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D3" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E3" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>249</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="E4" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D5" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E5" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>213</v>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>248</v>
+      </c>
+      <c r="B10" t="s">
+        <v>245</v>
+      </c>
+      <c r="C10" t="s">
+        <v>246</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -1463,6 +1517,8 @@
     <hyperlink ref="D8" r:id="rId2" xr:uid="{0E173CEE-01EF-4B92-9D17-89419912869D}"/>
     <hyperlink ref="E8" r:id="rId3" xr:uid="{3C908B1C-9AFF-4ABB-BD7C-25C46DA1A05F}"/>
     <hyperlink ref="E9" r:id="rId4" xr:uid="{63EB1EBB-F6AC-4CF6-8DAF-57743FA33772}"/>
+    <hyperlink ref="D10" r:id="rId5" xr:uid="{8CACEA37-D65D-480A-8C48-7A952734012D}"/>
+    <hyperlink ref="E10" r:id="rId6" xr:uid="{F5E659F7-59E8-45BA-8A48-DFCC9F3237A6}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1470,31 +1526,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62C3B9A7-7C48-4A5F-BA96-C7B5B0A75D9D}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>243</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+      <c r="D1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>247</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>248</v>
+        <v>260</v>
+      </c>
+      <c r="C2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -1503,11 +1565,60 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{296F9032-F396-446E-A1D2-198BE0C2AA62}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D2" t="s">
+        <v>241</v>
+      </c>
+      <c r="E2">
+        <v>2014</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FA83606-46F5-42E6-9D2B-9FE9A7C06680}">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C7" sqref="C7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1519,16 +1630,16 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1536,13 +1647,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1550,13 +1661,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1564,13 +1675,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1578,13 +1689,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1592,13 +1703,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
         <v>38</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1606,13 +1717,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>242</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>243</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1620,13 +1731,27 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>88</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1637,311 +1762,305 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BF54007-237F-4FC1-9763-EE9491EC144F}">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="10"/>
-    <col min="4" max="4" width="48.42578125" style="11" customWidth="1"/>
-    <col min="5" max="7" width="9.140625" style="10"/>
-    <col min="8" max="8" width="14.28515625" style="11" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="2" width="9.140625" style="10"/>
+    <col min="3" max="3" width="48.42578125" style="11" customWidth="1"/>
+    <col min="4" max="11" width="9.140625" style="10"/>
+    <col min="12" max="12" width="14.28515625" style="11" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A1" s="10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>98</v>
+        <v>31</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>93</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="P1" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>238</v>
-      </c>
       <c r="Q1" s="10" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="17.25" x14ac:dyDescent="0.4">
+        <v>255</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A2" s="10">
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="F2" s="10">
+        <v>215</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="10">
         <v>2024</v>
       </c>
-      <c r="G2" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="H2" t="s">
-        <v>127</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>232</v>
+      <c r="F2" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="L2" t="s">
+        <v>122</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>111</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="P2" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="17.25" x14ac:dyDescent="0.4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A3" s="10">
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="H3" t="s">
-        <v>128</v>
-      </c>
-      <c r="I3" t="s">
-        <v>118</v>
-      </c>
-      <c r="J3" t="s">
-        <v>118</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="17.25" x14ac:dyDescent="0.4">
+        <v>218</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="L3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M3" t="s">
+        <v>113</v>
+      </c>
+      <c r="N3" t="s">
+        <v>113</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A4" s="10">
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="F4" s="14">
+        <v>219</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="14">
         <v>2022</v>
       </c>
-      <c r="G4" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="H4" t="s">
-        <v>129</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="17.25" x14ac:dyDescent="0.4">
+      <c r="F4" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="L4" t="s">
+        <v>124</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A5" s="10">
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>117</v>
+        <v>216</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>118</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="H5" t="s">
-        <v>130</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="17.25" x14ac:dyDescent="0.4">
+        <v>129</v>
+      </c>
+      <c r="L5" t="s">
+        <v>125</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A6" s="10">
         <v>6</v>
       </c>
       <c r="B6" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" s="10">
+        <v>2019</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="L6" t="s">
+        <v>105</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="O6" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="F6" s="10">
-        <v>2019</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="H6" t="s">
-        <v>110</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="N6" s="10" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="17.25" x14ac:dyDescent="0.4">
+    </row>
+    <row r="7" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A7" s="10">
         <v>7</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="E7" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>119</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="H7" t="s">
-        <v>131</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="D9" s="12"/>
-    </row>
-    <row r="11" spans="1:17" ht="17.25" x14ac:dyDescent="0.4">
-      <c r="D11" s="9"/>
-      <c r="H11" s="10"/>
-      <c r="K11"/>
+        <v>127</v>
+      </c>
+      <c r="L7" t="s">
+        <v>126</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="C9" s="12"/>
+    </row>
+    <row r="11" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
+      <c r="C11" s="9"/>
+      <c r="L11" s="10"/>
+      <c r="O11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>
@@ -1949,12 +2068,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9D50774-E0FE-44E9-B03C-E8852FD49129}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1965,253 +2084,231 @@
     <col min="4" max="4" width="29.5703125" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37.140625" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:20" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="L1" t="s">
         <v>89</v>
       </c>
-      <c r="D1" t="s">
+      <c r="M1" t="s">
         <v>90</v>
       </c>
-      <c r="E1" t="s">
+      <c r="N1" t="s">
         <v>91</v>
       </c>
-      <c r="F1" t="s">
+      <c r="O1" t="s">
         <v>92</v>
       </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I1" t="s">
-        <v>94</v>
-      </c>
-      <c r="J1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K1" t="s">
-        <v>96</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="P1" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>256</v>
+      </c>
+      <c r="R1" t="s">
+        <v>257</v>
+      </c>
+      <c r="S1" t="s">
+        <v>258</v>
+      </c>
+      <c r="T1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="C2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D2" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>189</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="J2" t="s">
-        <v>52</v>
-      </c>
-      <c r="K2" t="s">
-        <v>190</v>
-      </c>
-      <c r="L2" t="s">
-        <v>240</v>
-      </c>
-      <c r="M2" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="N2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E3" s="2">
         <v>2020</v>
       </c>
       <c r="F3" t="s">
-        <v>206</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="J3" s="2">
+        <v>201</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="N3" s="2">
         <v>2020</v>
       </c>
-      <c r="K3" t="s">
-        <v>200</v>
-      </c>
-      <c r="L3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="O3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" t="s">
-        <v>201</v>
-      </c>
-      <c r="L4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="M4" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E5" s="2">
         <v>2017</v>
       </c>
       <c r="F5" t="s">
-        <v>205</v>
-      </c>
-      <c r="G5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>198</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="J5" s="2">
+        <v>200</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="N5" s="2">
         <v>2017</v>
       </c>
-      <c r="K5" t="s">
-        <v>202</v>
-      </c>
-      <c r="L5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>204</v>
-      </c>
-      <c r="G6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" t="s">
-        <v>203</v>
-      </c>
-      <c r="L6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L6" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E12" s="3"/>
     </row>
   </sheetData>
@@ -2219,11 +2316,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C521AE-7795-4323-919C-30CD2C445C0F}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -2234,16 +2331,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2254,10 +2351,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2268,10 +2365,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2282,10 +2379,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2296,10 +2393,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2310,10 +2407,10 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2324,10 +2421,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D7" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2338,10 +2435,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D8" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2352,10 +2449,10 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D9" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2366,10 +2463,10 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2380,10 +2477,10 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2394,10 +2491,10 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D12" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2408,10 +2505,10 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D13" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2422,10 +2519,10 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D14" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2436,10 +2533,10 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D15" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2450,10 +2547,10 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D16" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2464,10 +2561,10 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D17" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2478,10 +2575,10 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D18" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2492,10 +2589,10 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D19" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2506,10 +2603,10 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D20" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2520,10 +2617,10 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D21" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2534,10 +2631,10 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D22" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2548,10 +2645,10 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D23" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2562,10 +2659,10 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D24" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E24" s="3"/>
     </row>
@@ -2577,10 +2674,10 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D25" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2591,10 +2688,10 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D26" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2605,10 +2702,10 @@
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D27" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2619,10 +2716,10 @@
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D28" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2633,10 +2730,10 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D29" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2647,10 +2744,10 @@
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D30" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2661,10 +2758,10 @@
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D31" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2675,10 +2772,10 @@
         <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D32" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2689,10 +2786,10 @@
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D33" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2703,10 +2800,10 @@
         <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D34" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2717,10 +2814,10 @@
         <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D35" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2731,10 +2828,10 @@
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D36" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2745,10 +2842,10 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D37" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2759,10 +2856,10 @@
         <v>6</v>
       </c>
       <c r="C38" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D38" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -2773,10 +2870,10 @@
         <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D39" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2784,7 +2881,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E161CE-26B7-4F65-921B-3B054C05C05F}">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -2796,19 +2893,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2816,16 +2913,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2833,16 +2930,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2850,16 +2947,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2867,7 +2964,7 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2875,16 +2972,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2892,16 +2989,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2909,16 +3006,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" t="s">
         <v>77</v>
       </c>
-      <c r="C8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" t="s">
-        <v>81</v>
-      </c>
       <c r="E8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Criação dá página html que importa dados da planilha e permite a atualização da mesma
</commit_message>
<xml_diff>
--- a/dados_exemplo.xlsx
+++ b/dados_exemplo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GABRIEL\Documents\curriculo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C973BC45-9F69-461D-93A7-DEC2A3D60818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4AA1DA3-37EC-4EE8-A178-EDE89CA8C3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{8D5C2EF7-12FE-4554-BA32-BDC8432EB3A7}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="845" firstSheet="1" activeTab="6" xr2:uid="{8D5C2EF7-12FE-4554-BA32-BDC8432EB3A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Cabeçalho" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="262">
   <si>
     <t>Nome</t>
   </si>
@@ -826,6 +826,9 @@
   </si>
   <si>
     <t>main</t>
+  </si>
+  <si>
+    <t>grupo</t>
   </si>
 </sst>
 </file>
@@ -1332,7 +1335,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1528,8 +1531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62C3B9A7-7C48-4A5F-BA96-C7B5B0A75D9D}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1569,7 +1572,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1767,7 +1770,7 @@
   <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.4"/>
@@ -2073,7 +2076,7 @@
   <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2318,18 +2321,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C521AE-7795-4323-919C-30CD2C445C0F}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="2" max="3" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2337,542 +2340,552 @@
         <v>16</v>
       </c>
       <c r="C1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D1" t="s">
         <v>36</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>133</v>
+      <c r="C2" s="5" t="s">
+        <v>230</v>
       </c>
       <c r="D2" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
+      <c r="C3" s="5"/>
       <c r="D3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="5">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
-        <v>134</v>
-      </c>
+      <c r="C4" s="5"/>
       <c r="D4" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="5">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
-        <v>135</v>
-      </c>
+      <c r="C5" s="5"/>
       <c r="D5" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="5">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
+      <c r="C6" s="5"/>
       <c r="D6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7" t="s">
-        <v>136</v>
-      </c>
       <c r="D7" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
-      <c r="C8" t="s">
-        <v>137</v>
-      </c>
       <c r="D8" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
-      <c r="C9" t="s">
-        <v>138</v>
-      </c>
       <c r="D9" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
       <c r="D10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
       <c r="D11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
-      <c r="C12" t="s">
-        <v>139</v>
-      </c>
       <c r="D12" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
-      <c r="C13" t="s">
-        <v>140</v>
-      </c>
       <c r="D13" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
-      <c r="C14" t="s">
-        <v>141</v>
-      </c>
       <c r="D14" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
-      <c r="C15" t="s">
-        <v>142</v>
-      </c>
       <c r="D15" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
-      <c r="C16" t="s">
-        <v>143</v>
-      </c>
       <c r="D16" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
-      <c r="C17" t="s">
-        <v>144</v>
-      </c>
       <c r="D17" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
-      <c r="C18" t="s">
-        <v>145</v>
-      </c>
       <c r="D18" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
       <c r="B19">
         <v>3</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>146</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
       <c r="B20">
         <v>3</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>147</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>21</v>
       </c>
       <c r="B21">
         <v>3</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>148</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>22</v>
       </c>
       <c r="B22">
         <v>3</v>
       </c>
-      <c r="C22" t="s">
-        <v>149</v>
-      </c>
       <c r="D22" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>23</v>
       </c>
       <c r="B23">
         <v>3</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>150</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>24</v>
       </c>
       <c r="B24">
         <v>3</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>151</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>162</v>
       </c>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>25</v>
       </c>
       <c r="B25">
         <v>3</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>152</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>26</v>
       </c>
       <c r="B26">
         <v>3</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>153</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>27</v>
       </c>
       <c r="B27">
         <v>3</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>154</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>28</v>
       </c>
       <c r="B28">
         <v>3</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>155</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>29</v>
       </c>
       <c r="B29">
         <v>3</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>156</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>30</v>
       </c>
       <c r="B30">
         <v>3</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>157</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>31</v>
       </c>
       <c r="B31">
         <v>4</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>177</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>32</v>
       </c>
       <c r="B32">
         <v>4</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>178</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>33</v>
       </c>
       <c r="B33">
         <v>4</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>179</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>34</v>
       </c>
       <c r="B34">
         <v>4</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>180</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>35</v>
       </c>
       <c r="B35">
         <v>4</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>181</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>36</v>
       </c>
       <c r="B36">
         <v>4</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>182</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>37</v>
       </c>
       <c r="B37">
         <v>5</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>170</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>38</v>
       </c>
       <c r="B38">
         <v>6</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>81</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>39</v>
       </c>
       <c r="B39">
         <v>7</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>110</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2886,7 +2899,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2963,6 +2976,9 @@
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E5" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Criação do Fluxo de Usuários + Versões
</commit_message>
<xml_diff>
--- a/dados_exemplo.xlsx
+++ b/dados_exemplo.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GABRIEL\Documents\curriculo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4AA1DA3-37EC-4EE8-A178-EDE89CA8C3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0557D9-75B7-4F2A-A361-50860A4C765E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="845" firstSheet="1" activeTab="6" xr2:uid="{8D5C2EF7-12FE-4554-BA32-BDC8432EB3A7}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="845" firstSheet="2" activeTab="8" xr2:uid="{8D5C2EF7-12FE-4554-BA32-BDC8432EB3A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Cabeçalho" sheetId="1" r:id="rId1"/>
-    <sheet name="Resumo" sheetId="8" r:id="rId2"/>
-    <sheet name="Outros" sheetId="9" r:id="rId3"/>
-    <sheet name="Seções" sheetId="6" r:id="rId4"/>
-    <sheet name="Experiências" sheetId="2" r:id="rId5"/>
-    <sheet name="Formações" sheetId="3" r:id="rId6"/>
-    <sheet name="Habilidades" sheetId="4" r:id="rId7"/>
-    <sheet name="Classes" sheetId="7" r:id="rId8"/>
+    <sheet name="Títulos" sheetId="10" r:id="rId2"/>
+    <sheet name="Resumo" sheetId="8" r:id="rId3"/>
+    <sheet name="Outros" sheetId="9" r:id="rId4"/>
+    <sheet name="Seções" sheetId="6" r:id="rId5"/>
+    <sheet name="Experiências" sheetId="2" r:id="rId6"/>
+    <sheet name="Formações" sheetId="3" r:id="rId7"/>
+    <sheet name="Habilidades" sheetId="4" r:id="rId8"/>
+    <sheet name="Classes" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="260">
   <si>
     <t>Nome</t>
   </si>
@@ -225,9 +226,6 @@
     <t>MG, Brazil</t>
   </si>
   <si>
-    <t>Título</t>
-  </si>
-  <si>
     <t>Cidade</t>
   </si>
   <si>
@@ -243,9 +241,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
     <t>City</t>
   </si>
   <si>
@@ -792,43 +787,43 @@
     <t>url</t>
   </si>
   <si>
-    <t>titulo</t>
-  </si>
-  <si>
-    <t>detalhe_1_pt</t>
-  </si>
-  <si>
-    <t>detalhe_2_pt</t>
-  </si>
-  <si>
-    <t>detalhe_3_pt</t>
-  </si>
-  <si>
-    <t>detalhe_4_pt</t>
-  </si>
-  <si>
-    <t>detalhe_5_pt</t>
-  </si>
-  <si>
-    <t>detalhe_1_en</t>
-  </si>
-  <si>
-    <t>detalhe_2_en</t>
-  </si>
-  <si>
-    <t>detalhe_3_en</t>
-  </si>
-  <si>
-    <t>detalhe_4_en</t>
-  </si>
-  <si>
-    <t>detalhe_5_en</t>
-  </si>
-  <si>
     <t>main</t>
   </si>
   <si>
     <t>grupo</t>
+  </si>
+  <si>
+    <t>tit</t>
+  </si>
+  <si>
+    <t>detalhe1_pt</t>
+  </si>
+  <si>
+    <t>detalhe2_pt</t>
+  </si>
+  <si>
+    <t>detalhe3_pt</t>
+  </si>
+  <si>
+    <t>detalhe4_pt</t>
+  </si>
+  <si>
+    <t>detalhe5_pt</t>
+  </si>
+  <si>
+    <t>detalhe1_en</t>
+  </si>
+  <si>
+    <t>detalhe2_en</t>
+  </si>
+  <si>
+    <t>detalhe3_en</t>
+  </si>
+  <si>
+    <t>detalhe4_en</t>
+  </si>
+  <si>
+    <t>detalhe5_en</t>
   </si>
 </sst>
 </file>
@@ -975,7 +970,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -996,7 +991,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1332,10 +1326,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01DA8488-C559-41A8-B6D7-36686CD06534}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,10 +1343,10 @@
         <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D1" t="s">
         <v>57</v>
@@ -1369,165 +1363,191 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" t="s">
         <v>107</v>
       </c>
-      <c r="B3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" t="s">
-        <v>109</v>
-      </c>
       <c r="D3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>249</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>235</v>
+        <v>201</v>
       </c>
       <c r="E4" t="s">
-        <v>234</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>203</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>203</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>59</v>
+        <v>67</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>63</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>204</v>
+        <v>63</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>246</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>243</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>244</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>208</v>
+        <v>245</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>248</v>
-      </c>
-      <c r="B10" t="s">
         <v>245</v>
-      </c>
-      <c r="C10" t="s">
-        <v>246</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>247</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1" xr:uid="{32DE25E0-38CB-455D-AC5C-354A21B7E9BA}"/>
-    <hyperlink ref="D8" r:id="rId2" xr:uid="{0E173CEE-01EF-4B92-9D17-89419912869D}"/>
-    <hyperlink ref="E8" r:id="rId3" xr:uid="{3C908B1C-9AFF-4ABB-BD7C-25C46DA1A05F}"/>
-    <hyperlink ref="E9" r:id="rId4" xr:uid="{63EB1EBB-F6AC-4CF6-8DAF-57743FA33772}"/>
-    <hyperlink ref="D10" r:id="rId5" xr:uid="{8CACEA37-D65D-480A-8C48-7A952734012D}"/>
-    <hyperlink ref="E10" r:id="rId6" xr:uid="{F5E659F7-59E8-45BA-8A48-DFCC9F3237A6}"/>
+    <hyperlink ref="D8" r:id="rId1" xr:uid="{32DE25E0-38CB-455D-AC5C-354A21B7E9BA}"/>
+    <hyperlink ref="D7" r:id="rId2" xr:uid="{0E173CEE-01EF-4B92-9D17-89419912869D}"/>
+    <hyperlink ref="E7" r:id="rId3" xr:uid="{3C908B1C-9AFF-4ABB-BD7C-25C46DA1A05F}"/>
+    <hyperlink ref="E8" r:id="rId4" xr:uid="{63EB1EBB-F6AC-4CF6-8DAF-57743FA33772}"/>
+    <hyperlink ref="D9" r:id="rId5" xr:uid="{8CACEA37-D65D-480A-8C48-7A952734012D}"/>
+    <hyperlink ref="E9" r:id="rId6" xr:uid="{F5E659F7-59E8-45BA-8A48-DFCC9F3237A6}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6EC0001-0859-44A6-A7F2-A0D29E722D36}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62C3B9A7-7C48-4A5F-BA96-C7B5B0A75D9D}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1542,10 +1562,10 @@
         <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1553,13 +1573,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="C2" t="s">
-        <v>236</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>237</v>
+        <v>234</v>
+      </c>
+      <c r="D2" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -1567,7 +1587,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{296F9032-F396-446E-A1D2-198BE0C2AA62}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1585,13 +1605,13 @@
         <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1599,13 +1619,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D2" t="s">
         <v>239</v>
-      </c>
-      <c r="C2" t="s">
-        <v>240</v>
-      </c>
-      <c r="D2" t="s">
-        <v>241</v>
       </c>
       <c r="E2">
         <v>2014</v>
@@ -1616,7 +1636,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FA83606-46F5-42E6-9D2B-9FE9A7C06680}">
   <dimension ref="A1:H14"/>
   <sheetViews>
@@ -1664,7 +1684,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C3" t="s">
         <v>27</v>
@@ -1678,13 +1698,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" t="s">
         <v>99</v>
-      </c>
-      <c r="C4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1720,13 +1740,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>240</v>
+      </c>
+      <c r="C7" t="s">
+        <v>241</v>
+      </c>
+      <c r="D7" t="s">
         <v>242</v>
-      </c>
-      <c r="C7" t="s">
-        <v>243</v>
-      </c>
-      <c r="D7" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1748,13 +1768,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1765,12 +1785,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BF54007-237F-4FC1-9763-EE9491EC144F}">
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.4"/>
@@ -1790,16 +1810,16 @@
         <v>31</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>250</v>
@@ -1817,19 +1837,19 @@
         <v>254</v>
       </c>
       <c r="L1" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="P1" s="10" t="s">
         <v>95</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>97</v>
       </c>
       <c r="Q1" s="10" t="s">
         <v>255</v>
@@ -1852,40 +1872,40 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E2" s="10">
         <v>2024</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G2" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="J2" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="I2" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>229</v>
-      </c>
       <c r="L2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N2" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O2" s="10" t="s">
         <v>44</v>
@@ -1896,28 +1916,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="N3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="O3" s="10" t="s">
         <v>47</v>
@@ -1928,28 +1948,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E4" s="14">
         <v>2022</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N4" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="O4" s="10" t="s">
         <v>45</v>
@@ -1960,28 +1980,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="N5" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="O5" s="10" t="s">
         <v>46</v>
@@ -1992,37 +2012,37 @@
         <v>6</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E6" s="10">
         <v>2019</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="L6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M6" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="N6" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O6" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
@@ -2030,31 +2050,31 @@
         <v>7</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="M7" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="N7" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.4">
@@ -2071,12 +2091,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9D50774-E0FE-44E9-B03C-E8852FD49129}">
   <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2097,16 +2117,16 @@
         <v>31</v>
       </c>
       <c r="C1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" t="s">
         <v>85</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>86</v>
-      </c>
-      <c r="E1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F1" t="s">
-        <v>88</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>250</v>
@@ -2124,30 +2144,30 @@
         <v>254</v>
       </c>
       <c r="L1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N1" t="s">
         <v>89</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>90</v>
       </c>
-      <c r="N1" t="s">
-        <v>91</v>
-      </c>
-      <c r="O1" t="s">
-        <v>92</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="P1" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="10" t="s">
         <v>259</v>
       </c>
     </row>
@@ -2156,31 +2176,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
       </c>
       <c r="F2" t="s">
+        <v>182</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="M2" s="7" t="s">
         <v>184</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>186</v>
       </c>
       <c r="N2" t="s">
         <v>48</v>
       </c>
       <c r="O2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -2188,31 +2208,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E3" s="2">
         <v>2020</v>
       </c>
       <c r="F3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="N3" s="2">
         <v>2020</v>
       </c>
       <c r="O3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
@@ -2220,13 +2240,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
@@ -2235,16 +2255,16 @@
         <v>15</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="O4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -2252,31 +2272,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E5" s="2">
         <v>2017</v>
       </c>
       <c r="F5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N5" s="2">
         <v>2017</v>
       </c>
       <c r="O5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -2284,31 +2304,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="O6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -2319,12 +2339,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C521AE-7795-4323-919C-30CD2C445C0F}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2340,7 +2360,7 @@
         <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="D1" t="s">
         <v>36</v>
@@ -2357,13 +2377,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2390,10 +2410,10 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2405,10 +2425,10 @@
       </c>
       <c r="C5" s="5"/>
       <c r="D5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2434,10 +2454,10 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2448,10 +2468,10 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2462,10 +2482,10 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2504,10 +2524,10 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2518,10 +2538,10 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2532,10 +2552,10 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2546,10 +2566,10 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2560,10 +2580,10 @@
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2574,10 +2594,10 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2588,10 +2608,10 @@
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2602,10 +2622,10 @@
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2616,10 +2636,10 @@
         <v>3</v>
       </c>
       <c r="D20" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2630,10 +2650,10 @@
         <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E21" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2644,10 +2664,10 @@
         <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E22" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2658,10 +2678,10 @@
         <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E23" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2672,10 +2692,10 @@
         <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E24" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F24" s="3"/>
     </row>
@@ -2687,10 +2707,10 @@
         <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E25" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2701,10 +2721,10 @@
         <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E26" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2715,10 +2735,10 @@
         <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E27" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2729,10 +2749,10 @@
         <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2743,10 +2763,10 @@
         <v>3</v>
       </c>
       <c r="D29" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E29" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2757,10 +2777,10 @@
         <v>3</v>
       </c>
       <c r="D30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E30" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -2771,10 +2791,10 @@
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E31" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2785,10 +2805,10 @@
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E32" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2799,10 +2819,10 @@
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E33" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -2813,10 +2833,10 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E34" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2827,10 +2847,10 @@
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E35" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -2841,10 +2861,10 @@
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E36" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -2855,10 +2875,10 @@
         <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2869,10 +2889,10 @@
         <v>6</v>
       </c>
       <c r="D38" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E38" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2883,10 +2903,10 @@
         <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E39" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2894,19 +2914,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E161CE-26B7-4F65-921B-3B054C05C05F}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>31</v>
@@ -2988,13 +3006,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E6" t="s">
         <v>43</v>
@@ -3005,13 +3023,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" t="s">
         <v>73</v>
       </c>
-      <c r="C7" t="s">
-        <v>75</v>
-      </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
         <v>43</v>
@@ -3022,13 +3040,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E8" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Explicações dentro da página currículo sobre a localização de cada item na planilha e no arquivo modelo
</commit_message>
<xml_diff>
--- a/dados_exemplo.xlsx
+++ b/dados_exemplo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GABRIEL\Documents\curriculo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0557D9-75B7-4F2A-A361-50860A4C765E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D046CEE-3E2D-4106-BA0A-283E02EE9748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="845" firstSheet="2" activeTab="8" xr2:uid="{8D5C2EF7-12FE-4554-BA32-BDC8432EB3A7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="845" activeTab="7" xr2:uid="{8D5C2EF7-12FE-4554-BA32-BDC8432EB3A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Cabeçalho" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="263">
   <si>
     <t>Nome</t>
   </si>
@@ -142,12 +142,6 @@
     <t>alias</t>
   </si>
   <si>
-    <t>formacao</t>
-  </si>
-  <si>
-    <t>formacao_complementar</t>
-  </si>
-  <si>
     <t>habilidades_tecnicas</t>
   </si>
   <si>
@@ -824,6 +818,21 @@
   </si>
   <si>
     <t>detalhe5_en</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>formacoes</t>
+  </si>
+  <si>
+    <t>formacoes_complementares</t>
   </si>
 </sst>
 </file>
@@ -1332,30 +1341,30 @@
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
     <col min="4" max="4" width="74" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1363,132 +1372,132 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" t="s">
         <v>105</v>
       </c>
-      <c r="B3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C3" t="s">
-        <v>107</v>
-      </c>
       <c r="D3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B9" t="s">
+        <v>241</v>
+      </c>
+      <c r="C9" t="s">
+        <v>242</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="C9" t="s">
-        <v>244</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>245</v>
-      </c>
       <c r="E9" s="8" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -1512,9 +1521,9 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1522,24 +1531,24 @@
         <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -1555,31 +1564,31 @@
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -1595,9 +1604,9 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="16.2" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>10</v>
       </c>
@@ -1605,27 +1614,27 @@
         <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D2" t="s">
         <v>237</v>
-      </c>
-      <c r="C2" t="s">
-        <v>238</v>
-      </c>
-      <c r="D2" t="s">
-        <v>239</v>
       </c>
       <c r="E2">
         <v>2014</v>
@@ -1641,17 +1650,17 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:D7"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
+    <col min="3" max="3" width="39.6640625" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1659,125 +1668,125 @@
         <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>261</v>
       </c>
       <c r="C2" t="s">
         <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
         <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" t="s">
         <v>97</v>
       </c>
-      <c r="C4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>262</v>
       </c>
       <c r="C5" t="s">
         <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D7" t="s">
         <v>240</v>
       </c>
-      <c r="C7" t="s">
-        <v>241</v>
-      </c>
-      <c r="D7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
         <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H14" s="3"/>
     </row>
   </sheetData>
@@ -1790,19 +1799,19 @@
   <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:K1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.2" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="10"/>
-    <col min="3" max="3" width="48.42578125" style="11" customWidth="1"/>
-    <col min="4" max="11" width="9.140625" style="10"/>
-    <col min="12" max="12" width="14.28515625" style="11" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="2" width="9.109375" style="10"/>
+    <col min="3" max="3" width="48.44140625" style="11" customWidth="1"/>
+    <col min="4" max="11" width="9.109375" style="10"/>
+    <col min="12" max="12" width="14.33203125" style="11" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>10</v>
       </c>
@@ -1810,277 +1819,280 @@
         <v>31</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="M1" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>250</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="J1" s="10" t="s">
+      <c r="N1" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q1" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="R1" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="L1" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="T1" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="U1" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="T1" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="U1" s="10" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A2" s="10">
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E2" s="10">
         <v>2024</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G2" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="J2" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="K2" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="J2" s="10" t="s">
-        <v>227</v>
-      </c>
       <c r="L2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="N2" s="13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A3" s="10">
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="M3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A4" s="10">
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E4" s="14">
         <v>2022</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="L4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="N4" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A5" s="10">
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="N5" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="O5" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A6" s="10">
         <v>6</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E6" s="10">
         <v>2019</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="L6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="M6" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="N6" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="O6" s="10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7" s="10">
         <v>7</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M7" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="N7" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.4">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
       <c r="C9" s="12"/>
     </row>
-    <row r="11" spans="1:21" ht="17.25" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
       <c r="C11" s="9"/>
       <c r="L11" s="10"/>
       <c r="O11"/>
@@ -2095,21 +2107,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9D50774-E0FE-44E9-B03C-E8852FD49129}">
   <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:K1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="52.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="52.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.5546875" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.140625" customWidth="1"/>
+    <col min="6" max="6" width="37.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="17.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:20" ht="16.2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2117,136 +2129,151 @@
         <v>31</v>
       </c>
       <c r="C1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" t="s">
         <v>83</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>84</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="L1" t="s">
         <v>85</v>
       </c>
-      <c r="F1" t="s">
+      <c r="M1" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>250</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="J1" s="10" t="s">
+      <c r="N1" t="s">
+        <v>87</v>
+      </c>
+      <c r="O1" t="s">
+        <v>88</v>
+      </c>
+      <c r="P1" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="Q1" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="L1" t="s">
-        <v>87</v>
-      </c>
-      <c r="M1" t="s">
-        <v>88</v>
-      </c>
-      <c r="N1" t="s">
-        <v>89</v>
-      </c>
-      <c r="O1" t="s">
-        <v>90</v>
-      </c>
-      <c r="P1" s="10" t="s">
+      <c r="R1" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="T1" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="S1" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="T1" s="10" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
       </c>
       <c r="F2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G2" t="s">
+        <v>226</v>
+      </c>
+      <c r="H2" t="s">
+        <v>227</v>
+      </c>
+      <c r="I2" t="s">
+        <v>258</v>
+      </c>
+      <c r="J2" t="s">
+        <v>260</v>
+      </c>
+      <c r="K2" t="s">
+        <v>259</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="M2" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>184</v>
-      </c>
       <c r="N2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="O2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E3" s="2">
         <v>2020</v>
       </c>
       <c r="F3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="N3" s="2">
         <v>2020</v>
       </c>
       <c r="O3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
@@ -2255,83 +2282,83 @@
         <v>15</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="O4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E5" s="2">
         <v>2017</v>
       </c>
       <c r="F5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="N5" s="2">
         <v>2017</v>
       </c>
       <c r="O5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="O6" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="E12" s="3"/>
     </row>
   </sheetData>
@@ -2343,16 +2370,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C521AE-7795-4323-919C-30CD2C445C0F}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="16.7109375" customWidth="1"/>
+    <col min="2" max="3" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2360,16 +2387,16 @@
         <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2377,16 +2404,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2401,7 +2428,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2410,13 +2437,13 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2425,13 +2452,13 @@
       </c>
       <c r="C5" s="5"/>
       <c r="D5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2446,7 +2473,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2454,13 +2481,13 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2468,13 +2495,13 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2482,13 +2509,13 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2502,7 +2529,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2516,7 +2543,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2524,13 +2551,13 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E12" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2538,13 +2565,13 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E13" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2552,13 +2579,13 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2566,13 +2593,13 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E15" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2580,13 +2607,13 @@
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E16" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2594,13 +2621,13 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E17" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>18</v>
       </c>
@@ -2608,13 +2635,13 @@
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E18" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>19</v>
       </c>
@@ -2622,13 +2649,13 @@
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E19" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>20</v>
       </c>
@@ -2636,13 +2663,13 @@
         <v>3</v>
       </c>
       <c r="D20" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E20" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>21</v>
       </c>
@@ -2650,13 +2677,13 @@
         <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E21" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>22</v>
       </c>
@@ -2664,13 +2691,13 @@
         <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E22" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>23</v>
       </c>
@@ -2678,13 +2705,13 @@
         <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E23" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>24</v>
       </c>
@@ -2692,14 +2719,14 @@
         <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E24" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>25</v>
       </c>
@@ -2707,13 +2734,13 @@
         <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E25" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>26</v>
       </c>
@@ -2721,13 +2748,13 @@
         <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E26" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>27</v>
       </c>
@@ -2735,13 +2762,13 @@
         <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E27" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>28</v>
       </c>
@@ -2749,13 +2776,13 @@
         <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E28" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>29</v>
       </c>
@@ -2763,13 +2790,13 @@
         <v>3</v>
       </c>
       <c r="D29" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E29" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>30</v>
       </c>
@@ -2777,27 +2804,30 @@
         <v>3</v>
       </c>
       <c r="D30" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E30" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>31</v>
       </c>
       <c r="B31">
         <v>4</v>
       </c>
+      <c r="C31" t="s">
+        <v>227</v>
+      </c>
       <c r="D31" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E31" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>32</v>
       </c>
@@ -2805,13 +2835,13 @@
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E32" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>33</v>
       </c>
@@ -2819,13 +2849,13 @@
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E33" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>34</v>
       </c>
@@ -2833,13 +2863,13 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E34" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>35</v>
       </c>
@@ -2847,13 +2877,13 @@
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E35" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>36</v>
       </c>
@@ -2861,27 +2891,30 @@
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E36" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>37</v>
       </c>
       <c r="B37">
         <v>5</v>
       </c>
+      <c r="C37" t="s">
+        <v>258</v>
+      </c>
       <c r="D37" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E37" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>38</v>
       </c>
@@ -2889,13 +2922,13 @@
         <v>6</v>
       </c>
       <c r="D38" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E38" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>39</v>
       </c>
@@ -2903,10 +2936,10 @@
         <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E39" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2918,11 +2951,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E161CE-26B7-4F65-921B-3B054C05C05F}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2930,67 +2963,67 @@
         <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
         <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3001,58 +3034,58 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" t="s">
         <v>71</v>
       </c>
-      <c r="C7" t="s">
-        <v>73</v>
-      </c>
       <c r="D7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D9" s="3"/>
     </row>
   </sheetData>

</xml_diff>